<commit_message>
Working on generating_fake_data and stat_functions
</commit_message>
<xml_diff>
--- a/logs/Enrollment_Log.xlsx
+++ b/logs/Enrollment_Log.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="829">
   <si>
     <t>Subject_ID</t>
   </si>
@@ -1358,6 +1358,1152 @@
   </si>
   <si>
     <t>iwk</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>4/3/2016</t>
+  </si>
+  <si>
+    <t>6:11</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>wly</t>
+  </si>
+  <si>
+    <t>523</t>
+  </si>
+  <si>
+    <t>9/19/2014</t>
+  </si>
+  <si>
+    <t>14:28</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>cst</t>
+  </si>
+  <si>
+    <t>481</t>
+  </si>
+  <si>
+    <t>12/19/2014</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>fyw</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>1/18/2015</t>
+  </si>
+  <si>
+    <t>1:46</t>
+  </si>
+  <si>
+    <t>xdf</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>6/28/2015</t>
+  </si>
+  <si>
+    <t>9:33</t>
+  </si>
+  <si>
+    <t>dzs</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>7/9/2012</t>
+  </si>
+  <si>
+    <t>21:41</t>
+  </si>
+  <si>
+    <t>cwk</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
+    <t>1/6/2014</t>
+  </si>
+  <si>
+    <t>22:51</t>
+  </si>
+  <si>
+    <t>ynp</t>
+  </si>
+  <si>
+    <t>7/23/2016</t>
+  </si>
+  <si>
+    <t>6:27</t>
+  </si>
+  <si>
+    <t>bwe</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>4/27/2012</t>
+  </si>
+  <si>
+    <t>19:37</t>
+  </si>
+  <si>
+    <t>qav</t>
+  </si>
+  <si>
+    <t>768</t>
+  </si>
+  <si>
+    <t>7/2/2014</t>
+  </si>
+  <si>
+    <t>3:37</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>bqh</t>
+  </si>
+  <si>
+    <t>624</t>
+  </si>
+  <si>
+    <t>2/10/2015</t>
+  </si>
+  <si>
+    <t>11:56</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>rgm</t>
+  </si>
+  <si>
+    <t>816</t>
+  </si>
+  <si>
+    <t>12/13/2016</t>
+  </si>
+  <si>
+    <t>20:34</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>oej</t>
+  </si>
+  <si>
+    <t>327</t>
+  </si>
+  <si>
+    <t>12/24/2014</t>
+  </si>
+  <si>
+    <t>xph</t>
+  </si>
+  <si>
+    <t>786</t>
+  </si>
+  <si>
+    <t>4/20/2013</t>
+  </si>
+  <si>
+    <t>12:25</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>vny</t>
+  </si>
+  <si>
+    <t>485</t>
+  </si>
+  <si>
+    <t>9/22/2013</t>
+  </si>
+  <si>
+    <t>2:47</t>
+  </si>
+  <si>
+    <t>qhn</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>1/21/2015</t>
+  </si>
+  <si>
+    <t>21:11</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>nho</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10/24/2016</t>
+  </si>
+  <si>
+    <t>13:6</t>
+  </si>
+  <si>
+    <t>lef</t>
+  </si>
+  <si>
+    <t>566</t>
+  </si>
+  <si>
+    <t>8/17/2012</t>
+  </si>
+  <si>
+    <t>22:48</t>
+  </si>
+  <si>
+    <t>zqs</t>
+  </si>
+  <si>
+    <t>1/26/2016</t>
+  </si>
+  <si>
+    <t>9:21</t>
+  </si>
+  <si>
+    <t>mph</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t>4/13/2015</t>
+  </si>
+  <si>
+    <t>7:58</t>
+  </si>
+  <si>
+    <t>pdz</t>
+  </si>
+  <si>
+    <t>927</t>
+  </si>
+  <si>
+    <t>4/16/2015</t>
+  </si>
+  <si>
+    <t>3:2</t>
+  </si>
+  <si>
+    <t>tzu</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>12/11/2013</t>
+  </si>
+  <si>
+    <t>20:12</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>jqw</t>
+  </si>
+  <si>
+    <t>7/10/2013</t>
+  </si>
+  <si>
+    <t>21:53</t>
+  </si>
+  <si>
+    <t>bam</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>10/4/2013</t>
+  </si>
+  <si>
+    <t>13:2</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>jhx</t>
+  </si>
+  <si>
+    <t>2/18/2016</t>
+  </si>
+  <si>
+    <t>20:13</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>lyk</t>
+  </si>
+  <si>
+    <t>561</t>
+  </si>
+  <si>
+    <t>3/20/2015</t>
+  </si>
+  <si>
+    <t>18:43</t>
+  </si>
+  <si>
+    <t>cuu</t>
+  </si>
+  <si>
+    <t>1/23/2012</t>
+  </si>
+  <si>
+    <t>19:55</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>qfm</t>
+  </si>
+  <si>
+    <t>492</t>
+  </si>
+  <si>
+    <t>9/8/2012</t>
+  </si>
+  <si>
+    <t>18:12</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>pmq</t>
+  </si>
+  <si>
+    <t>7/24/2013</t>
+  </si>
+  <si>
+    <t>23:37</t>
+  </si>
+  <si>
+    <t>vae</t>
+  </si>
+  <si>
+    <t>905</t>
+  </si>
+  <si>
+    <t>6/16/2013</t>
+  </si>
+  <si>
+    <t>4:49</t>
+  </si>
+  <si>
+    <t>ars</t>
+  </si>
+  <si>
+    <t>856</t>
+  </si>
+  <si>
+    <t>9/27/2015</t>
+  </si>
+  <si>
+    <t>3:11</t>
+  </si>
+  <si>
+    <t>gpn</t>
+  </si>
+  <si>
+    <t>627</t>
+  </si>
+  <si>
+    <t>6/9/2015</t>
+  </si>
+  <si>
+    <t>0:26</t>
+  </si>
+  <si>
+    <t>gna</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1/3/2013</t>
+  </si>
+  <si>
+    <t>19:35</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>azq</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>1/23/2016</t>
+  </si>
+  <si>
+    <t>10:4</t>
+  </si>
+  <si>
+    <t>pgu</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>12/25/2013</t>
+  </si>
+  <si>
+    <t>14:3</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>rci</t>
+  </si>
+  <si>
+    <t>942</t>
+  </si>
+  <si>
+    <t>2/2/2012</t>
+  </si>
+  <si>
+    <t>7:22</t>
+  </si>
+  <si>
+    <t>elp</t>
+  </si>
+  <si>
+    <t>822</t>
+  </si>
+  <si>
+    <t>12/4/2014</t>
+  </si>
+  <si>
+    <t>17:37</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>ybf</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>3:34</t>
+  </si>
+  <si>
+    <t>ihk</t>
+  </si>
+  <si>
+    <t>874</t>
+  </si>
+  <si>
+    <t>18:4</t>
+  </si>
+  <si>
+    <t>dcr</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>1/23/2014</t>
+  </si>
+  <si>
+    <t>8:6</t>
+  </si>
+  <si>
+    <t>ols</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>3/7/2015</t>
+  </si>
+  <si>
+    <t>9:0</t>
+  </si>
+  <si>
+    <t>uzw</t>
+  </si>
+  <si>
+    <t>342</t>
+  </si>
+  <si>
+    <t>11/16/2014</t>
+  </si>
+  <si>
+    <t>16:52</t>
+  </si>
+  <si>
+    <t>qfr</t>
+  </si>
+  <si>
+    <t>570</t>
+  </si>
+  <si>
+    <t>10/23/2013</t>
+  </si>
+  <si>
+    <t>23:54</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>cnr</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>4/4/2012</t>
+  </si>
+  <si>
+    <t>21:49</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>gam</t>
+  </si>
+  <si>
+    <t>901</t>
+  </si>
+  <si>
+    <t>4/13/2012</t>
+  </si>
+  <si>
+    <t>6:54</t>
+  </si>
+  <si>
+    <t>hif</t>
+  </si>
+  <si>
+    <t>9/18/2016</t>
+  </si>
+  <si>
+    <t>2:30</t>
+  </si>
+  <si>
+    <t>wmd</t>
+  </si>
+  <si>
+    <t>591</t>
+  </si>
+  <si>
+    <t>5/12/2014</t>
+  </si>
+  <si>
+    <t>18:54</t>
+  </si>
+  <si>
+    <t>rhn</t>
+  </si>
+  <si>
+    <t>918</t>
+  </si>
+  <si>
+    <t>5/6/2013</t>
+  </si>
+  <si>
+    <t>884</t>
+  </si>
+  <si>
+    <t>11/23/2013</t>
+  </si>
+  <si>
+    <t>23:3</t>
+  </si>
+  <si>
+    <t>zwd</t>
+  </si>
+  <si>
+    <t>557</t>
+  </si>
+  <si>
+    <t>8/11/2013</t>
+  </si>
+  <si>
+    <t>20:17</t>
+  </si>
+  <si>
+    <t>yqu</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>5/15/2016</t>
+  </si>
+  <si>
+    <t>lvs</t>
+  </si>
+  <si>
+    <t>978</t>
+  </si>
+  <si>
+    <t>4/10/2014</t>
+  </si>
+  <si>
+    <t>8:5</t>
+  </si>
+  <si>
+    <t>fdx</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>12/4/2015</t>
+  </si>
+  <si>
+    <t>ffm</t>
+  </si>
+  <si>
+    <t>932</t>
+  </si>
+  <si>
+    <t>5/21/2015</t>
+  </si>
+  <si>
+    <t>9:56</t>
+  </si>
+  <si>
+    <t>kur</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>20:11</t>
+  </si>
+  <si>
+    <t>ohr</t>
+  </si>
+  <si>
+    <t>1/6/2015</t>
+  </si>
+  <si>
+    <t>7:17</t>
+  </si>
+  <si>
+    <t>bxj</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>4/5/2012</t>
+  </si>
+  <si>
+    <t>23:20</t>
+  </si>
+  <si>
+    <t>ncv</t>
+  </si>
+  <si>
+    <t>972</t>
+  </si>
+  <si>
+    <t>7/27/2016</t>
+  </si>
+  <si>
+    <t>cku</t>
+  </si>
+  <si>
+    <t>12/18/2013</t>
+  </si>
+  <si>
+    <t>23:31</t>
+  </si>
+  <si>
+    <t>gcv</t>
+  </si>
+  <si>
+    <t>422</t>
+  </si>
+  <si>
+    <t>1/5/2016</t>
+  </si>
+  <si>
+    <t>17:50</t>
+  </si>
+  <si>
+    <t>ofm</t>
+  </si>
+  <si>
+    <t>16:1</t>
+  </si>
+  <si>
+    <t>otl</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>9/8/2015</t>
+  </si>
+  <si>
+    <t>5:2</t>
+  </si>
+  <si>
+    <t>qnn</t>
+  </si>
+  <si>
+    <t>5/20/2013</t>
+  </si>
+  <si>
+    <t>7:55</t>
+  </si>
+  <si>
+    <t>bia</t>
+  </si>
+  <si>
+    <t>12/8/2012</t>
+  </si>
+  <si>
+    <t>23:42</t>
+  </si>
+  <si>
+    <t>rkv</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>9/9/2012</t>
+  </si>
+  <si>
+    <t>23:30</t>
+  </si>
+  <si>
+    <t>ozo</t>
+  </si>
+  <si>
+    <t>6/20/2016</t>
+  </si>
+  <si>
+    <t>4:27</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>3/8/2012</t>
+  </si>
+  <si>
+    <t>1:27</t>
+  </si>
+  <si>
+    <t>nqx</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>6/10/2016</t>
+  </si>
+  <si>
+    <t>18:11</t>
+  </si>
+  <si>
+    <t>oag</t>
+  </si>
+  <si>
+    <t>0:32</t>
+  </si>
+  <si>
+    <t>kue</t>
+  </si>
+  <si>
+    <t>946</t>
+  </si>
+  <si>
+    <t>11/16/2015</t>
+  </si>
+  <si>
+    <t>14:35</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>gwf</t>
+  </si>
+  <si>
+    <t>382</t>
+  </si>
+  <si>
+    <t>6/25/2014</t>
+  </si>
+  <si>
+    <t>9:22</t>
+  </si>
+  <si>
+    <t>qkb</t>
+  </si>
+  <si>
+    <t>921</t>
+  </si>
+  <si>
+    <t>9/12/2016</t>
+  </si>
+  <si>
+    <t>17:59</t>
+  </si>
+  <si>
+    <t>ukg</t>
+  </si>
+  <si>
+    <t>2/4/2015</t>
+  </si>
+  <si>
+    <t>8:45</t>
+  </si>
+  <si>
+    <t>hfi</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>2/21/2012</t>
+  </si>
+  <si>
+    <t>22:44</t>
+  </si>
+  <si>
+    <t>vfu</t>
+  </si>
+  <si>
+    <t>324</t>
+  </si>
+  <si>
+    <t>8/1/2015</t>
+  </si>
+  <si>
+    <t>5:43</t>
+  </si>
+  <si>
+    <t>gin</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>1:3</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>ckw</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
+    <t>7/8/2012</t>
+  </si>
+  <si>
+    <t>10:14</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>hyp</t>
+  </si>
+  <si>
+    <t>6/17/2016</t>
+  </si>
+  <si>
+    <t>12:9</t>
+  </si>
+  <si>
+    <t>iyo</t>
+  </si>
+  <si>
+    <t>931</t>
+  </si>
+  <si>
+    <t>21:31</t>
+  </si>
+  <si>
+    <t>wsl</t>
+  </si>
+  <si>
+    <t>405</t>
+  </si>
+  <si>
+    <t>8/28/2016</t>
+  </si>
+  <si>
+    <t>8:13</t>
+  </si>
+  <si>
+    <t>bpr</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>5/2/2013</t>
+  </si>
+  <si>
+    <t>5:0</t>
+  </si>
+  <si>
+    <t>kbp</t>
+  </si>
+  <si>
+    <t>797</t>
+  </si>
+  <si>
+    <t>8/14/2015</t>
+  </si>
+  <si>
+    <t>9:39</t>
+  </si>
+  <si>
+    <t>evy</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>10/20/2014</t>
+  </si>
+  <si>
+    <t>23:51</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>ljd</t>
+  </si>
+  <si>
+    <t>7/19/2015</t>
+  </si>
+  <si>
+    <t>15:58</t>
+  </si>
+  <si>
+    <t>pba</t>
+  </si>
+  <si>
+    <t>902</t>
+  </si>
+  <si>
+    <t>5/3/2012</t>
+  </si>
+  <si>
+    <t>22:15</t>
+  </si>
+  <si>
+    <t>bbn</t>
+  </si>
+  <si>
+    <t>5:18</t>
+  </si>
+  <si>
+    <t>ajj</t>
+  </si>
+  <si>
+    <t>878</t>
+  </si>
+  <si>
+    <t>14:8</t>
+  </si>
+  <si>
+    <t>dkh</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>12/5/2012</t>
+  </si>
+  <si>
+    <t>20:15</t>
+  </si>
+  <si>
+    <t>nmg</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>5/5/2014</t>
+  </si>
+  <si>
+    <t>15:35</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>pyi</t>
+  </si>
+  <si>
+    <t>387</t>
+  </si>
+  <si>
+    <t>4/7/2012</t>
+  </si>
+  <si>
+    <t>11:33</t>
+  </si>
+  <si>
+    <t>xky</t>
+  </si>
+  <si>
+    <t>573</t>
+  </si>
+  <si>
+    <t>3/27/2015</t>
+  </si>
+  <si>
+    <t>ckl</t>
+  </si>
+  <si>
+    <t>341</t>
+  </si>
+  <si>
+    <t>11/9/2016</t>
+  </si>
+  <si>
+    <t>lqn</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>15:37</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>dgk</t>
+  </si>
+  <si>
+    <t>681</t>
+  </si>
+  <si>
+    <t>8:31</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>5/1/2014</t>
+  </si>
+  <si>
+    <t>ugn</t>
+  </si>
+  <si>
+    <t>909</t>
+  </si>
+  <si>
+    <t>7/22/2013</t>
+  </si>
+  <si>
+    <t>dlz</t>
+  </si>
+  <si>
+    <t>554</t>
+  </si>
+  <si>
+    <t>4/4/2013</t>
+  </si>
+  <si>
+    <t>13:13</t>
+  </si>
+  <si>
+    <t>ncn</t>
+  </si>
+  <si>
+    <t>496</t>
+  </si>
+  <si>
+    <t>12/26/2015</t>
+  </si>
+  <si>
+    <t>hsy</t>
+  </si>
+  <si>
+    <t>339</t>
+  </si>
+  <si>
+    <t>5/5/2013</t>
+  </si>
+  <si>
+    <t>12:40</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>qoj</t>
+  </si>
+  <si>
+    <t>631</t>
+  </si>
+  <si>
+    <t>10/1/2013</t>
+  </si>
+  <si>
+    <t>2:11</t>
+  </si>
+  <si>
+    <t>als</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +2870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="2:10"/>
@@ -4062,6 +5208,2306 @@
       </c>
       <c r="G101" t="s">
         <v>446</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>447</v>
+      </c>
+      <c r="B102" t="s">
+        <v>448</v>
+      </c>
+      <c r="C102" t="s">
+        <v>449</v>
+      </c>
+      <c r="D102" t="s">
+        <v>450</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>452</v>
+      </c>
+      <c r="B103" t="s">
+        <v>453</v>
+      </c>
+      <c r="C103" t="s">
+        <v>454</v>
+      </c>
+      <c r="D103" t="s">
+        <v>455</v>
+      </c>
+      <c r="E103" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>457</v>
+      </c>
+      <c r="B104" t="s">
+        <v>458</v>
+      </c>
+      <c r="C104" t="s">
+        <v>449</v>
+      </c>
+      <c r="D104" t="s">
+        <v>459</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>461</v>
+      </c>
+      <c r="B105" t="s">
+        <v>462</v>
+      </c>
+      <c r="C105" t="s">
+        <v>463</v>
+      </c>
+      <c r="D105" t="s">
+        <v>138</v>
+      </c>
+      <c r="E105" t="s">
+        <v>18</v>
+      </c>
+      <c r="F105" t="s">
+        <v>30</v>
+      </c>
+      <c r="G105" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>465</v>
+      </c>
+      <c r="B106" t="s">
+        <v>466</v>
+      </c>
+      <c r="C106" t="s">
+        <v>467</v>
+      </c>
+      <c r="D106" t="s">
+        <v>155</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>469</v>
+      </c>
+      <c r="B107" t="s">
+        <v>470</v>
+      </c>
+      <c r="C107" t="s">
+        <v>471</v>
+      </c>
+      <c r="D107" t="s">
+        <v>279</v>
+      </c>
+      <c r="E107" t="s">
+        <v>24</v>
+      </c>
+      <c r="F107" t="s">
+        <v>30</v>
+      </c>
+      <c r="G107" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>473</v>
+      </c>
+      <c r="B108" t="s">
+        <v>474</v>
+      </c>
+      <c r="C108" t="s">
+        <v>475</v>
+      </c>
+      <c r="D108" t="s">
+        <v>331</v>
+      </c>
+      <c r="E108" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>318</v>
+      </c>
+      <c r="B109" t="s">
+        <v>477</v>
+      </c>
+      <c r="C109" t="s">
+        <v>478</v>
+      </c>
+      <c r="D109" t="s">
+        <v>59</v>
+      </c>
+      <c r="E109" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>480</v>
+      </c>
+      <c r="B110" t="s">
+        <v>481</v>
+      </c>
+      <c r="C110" t="s">
+        <v>482</v>
+      </c>
+      <c r="D110" t="s">
+        <v>250</v>
+      </c>
+      <c r="E110" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" t="s">
+        <v>30</v>
+      </c>
+      <c r="G110" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>484</v>
+      </c>
+      <c r="B111" t="s">
+        <v>485</v>
+      </c>
+      <c r="C111" t="s">
+        <v>486</v>
+      </c>
+      <c r="D111" t="s">
+        <v>487</v>
+      </c>
+      <c r="E111" t="s">
+        <v>24</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>489</v>
+      </c>
+      <c r="B112" t="s">
+        <v>490</v>
+      </c>
+      <c r="C112" t="s">
+        <v>491</v>
+      </c>
+      <c r="D112" t="s">
+        <v>492</v>
+      </c>
+      <c r="E112" t="s">
+        <v>18</v>
+      </c>
+      <c r="F112" t="s">
+        <v>30</v>
+      </c>
+      <c r="G112" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>494</v>
+      </c>
+      <c r="B113" t="s">
+        <v>495</v>
+      </c>
+      <c r="C113" t="s">
+        <v>496</v>
+      </c>
+      <c r="D113" t="s">
+        <v>497</v>
+      </c>
+      <c r="E113" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" t="s">
+        <v>30</v>
+      </c>
+      <c r="G113" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>499</v>
+      </c>
+      <c r="B114" t="s">
+        <v>500</v>
+      </c>
+      <c r="C114" t="s">
+        <v>182</v>
+      </c>
+      <c r="D114" t="s">
+        <v>17</v>
+      </c>
+      <c r="E114" t="s">
+        <v>18</v>
+      </c>
+      <c r="F114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>502</v>
+      </c>
+      <c r="B115" t="s">
+        <v>503</v>
+      </c>
+      <c r="C115" t="s">
+        <v>504</v>
+      </c>
+      <c r="D115" t="s">
+        <v>505</v>
+      </c>
+      <c r="E115" t="s">
+        <v>24</v>
+      </c>
+      <c r="F115" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>507</v>
+      </c>
+      <c r="B116" t="s">
+        <v>508</v>
+      </c>
+      <c r="C116" t="s">
+        <v>509</v>
+      </c>
+      <c r="D116" t="s">
+        <v>64</v>
+      </c>
+      <c r="E116" t="s">
+        <v>18</v>
+      </c>
+      <c r="F116" t="s">
+        <v>30</v>
+      </c>
+      <c r="G116" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>511</v>
+      </c>
+      <c r="B117" t="s">
+        <v>512</v>
+      </c>
+      <c r="C117" t="s">
+        <v>513</v>
+      </c>
+      <c r="D117" t="s">
+        <v>514</v>
+      </c>
+      <c r="E117" t="s">
+        <v>24</v>
+      </c>
+      <c r="F117" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>516</v>
+      </c>
+      <c r="B118" t="s">
+        <v>517</v>
+      </c>
+      <c r="C118" t="s">
+        <v>518</v>
+      </c>
+      <c r="D118" t="s">
+        <v>403</v>
+      </c>
+      <c r="E118" t="s">
+        <v>24</v>
+      </c>
+      <c r="F118" t="s">
+        <v>30</v>
+      </c>
+      <c r="G118" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>520</v>
+      </c>
+      <c r="B119" t="s">
+        <v>521</v>
+      </c>
+      <c r="C119" t="s">
+        <v>522</v>
+      </c>
+      <c r="D119" t="s">
+        <v>148</v>
+      </c>
+      <c r="E119" t="s">
+        <v>24</v>
+      </c>
+      <c r="F119" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120" t="s">
+        <v>524</v>
+      </c>
+      <c r="C120" t="s">
+        <v>525</v>
+      </c>
+      <c r="D120" t="s">
+        <v>169</v>
+      </c>
+      <c r="E120" t="s">
+        <v>18</v>
+      </c>
+      <c r="F120" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>527</v>
+      </c>
+      <c r="B121" t="s">
+        <v>528</v>
+      </c>
+      <c r="C121" t="s">
+        <v>529</v>
+      </c>
+      <c r="D121" t="s">
+        <v>364</v>
+      </c>
+      <c r="E121" t="s">
+        <v>18</v>
+      </c>
+      <c r="F121" t="s">
+        <v>30</v>
+      </c>
+      <c r="G121" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>531</v>
+      </c>
+      <c r="B122" t="s">
+        <v>532</v>
+      </c>
+      <c r="C122" t="s">
+        <v>533</v>
+      </c>
+      <c r="D122" t="s">
+        <v>157</v>
+      </c>
+      <c r="E122" t="s">
+        <v>24</v>
+      </c>
+      <c r="F122" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>535</v>
+      </c>
+      <c r="B123" t="s">
+        <v>536</v>
+      </c>
+      <c r="C123" t="s">
+        <v>537</v>
+      </c>
+      <c r="D123" t="s">
+        <v>538</v>
+      </c>
+      <c r="E123" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" t="s">
+        <v>30</v>
+      </c>
+      <c r="G123" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>201</v>
+      </c>
+      <c r="B124" t="s">
+        <v>540</v>
+      </c>
+      <c r="C124" t="s">
+        <v>541</v>
+      </c>
+      <c r="D124" t="s">
+        <v>313</v>
+      </c>
+      <c r="E124" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>543</v>
+      </c>
+      <c r="B125" t="s">
+        <v>544</v>
+      </c>
+      <c r="C125" t="s">
+        <v>545</v>
+      </c>
+      <c r="D125" t="s">
+        <v>546</v>
+      </c>
+      <c r="E125" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" t="s">
+        <v>12</v>
+      </c>
+      <c r="G125" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>93</v>
+      </c>
+      <c r="B126" t="s">
+        <v>548</v>
+      </c>
+      <c r="C126" t="s">
+        <v>549</v>
+      </c>
+      <c r="D126" t="s">
+        <v>550</v>
+      </c>
+      <c r="E126" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" t="s">
+        <v>30</v>
+      </c>
+      <c r="G126" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>552</v>
+      </c>
+      <c r="B127" t="s">
+        <v>553</v>
+      </c>
+      <c r="C127" t="s">
+        <v>554</v>
+      </c>
+      <c r="D127" t="s">
+        <v>212</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>455</v>
+      </c>
+      <c r="B128" t="s">
+        <v>556</v>
+      </c>
+      <c r="C128" t="s">
+        <v>557</v>
+      </c>
+      <c r="D128" t="s">
+        <v>558</v>
+      </c>
+      <c r="E128" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" t="s">
+        <v>12</v>
+      </c>
+      <c r="G128" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>560</v>
+      </c>
+      <c r="B129" t="s">
+        <v>561</v>
+      </c>
+      <c r="C129" t="s">
+        <v>562</v>
+      </c>
+      <c r="D129" t="s">
+        <v>563</v>
+      </c>
+      <c r="E129" t="s">
+        <v>24</v>
+      </c>
+      <c r="F129" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>318</v>
+      </c>
+      <c r="B130" t="s">
+        <v>565</v>
+      </c>
+      <c r="C130" t="s">
+        <v>566</v>
+      </c>
+      <c r="D130" t="s">
+        <v>248</v>
+      </c>
+      <c r="E130" t="s">
+        <v>24</v>
+      </c>
+      <c r="F130" t="s">
+        <v>30</v>
+      </c>
+      <c r="G130" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>568</v>
+      </c>
+      <c r="B131" t="s">
+        <v>569</v>
+      </c>
+      <c r="C131" t="s">
+        <v>570</v>
+      </c>
+      <c r="D131" t="s">
+        <v>45</v>
+      </c>
+      <c r="E131" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" t="s">
+        <v>30</v>
+      </c>
+      <c r="G131" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>572</v>
+      </c>
+      <c r="B132" t="s">
+        <v>573</v>
+      </c>
+      <c r="C132" t="s">
+        <v>574</v>
+      </c>
+      <c r="D132" t="s">
+        <v>45</v>
+      </c>
+      <c r="E132" t="s">
+        <v>18</v>
+      </c>
+      <c r="F132" t="s">
+        <v>30</v>
+      </c>
+      <c r="G132" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
+        <v>576</v>
+      </c>
+      <c r="B133" t="s">
+        <v>577</v>
+      </c>
+      <c r="C133" t="s">
+        <v>578</v>
+      </c>
+      <c r="D133" t="s">
+        <v>109</v>
+      </c>
+      <c r="E133" t="s">
+        <v>18</v>
+      </c>
+      <c r="F133" t="s">
+        <v>12</v>
+      </c>
+      <c r="G133" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
+        <v>580</v>
+      </c>
+      <c r="B134" t="s">
+        <v>581</v>
+      </c>
+      <c r="C134" t="s">
+        <v>582</v>
+      </c>
+      <c r="D134" t="s">
+        <v>583</v>
+      </c>
+      <c r="E134" t="s">
+        <v>24</v>
+      </c>
+      <c r="F134" t="s">
+        <v>12</v>
+      </c>
+      <c r="G134" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
+        <v>585</v>
+      </c>
+      <c r="B135" t="s">
+        <v>586</v>
+      </c>
+      <c r="C135" t="s">
+        <v>587</v>
+      </c>
+      <c r="D135" t="s">
+        <v>279</v>
+      </c>
+      <c r="E135" t="s">
+        <v>18</v>
+      </c>
+      <c r="F135" t="s">
+        <v>12</v>
+      </c>
+      <c r="G135" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>589</v>
+      </c>
+      <c r="B136" t="s">
+        <v>590</v>
+      </c>
+      <c r="C136" t="s">
+        <v>591</v>
+      </c>
+      <c r="D136" t="s">
+        <v>592</v>
+      </c>
+      <c r="E136" t="s">
+        <v>24</v>
+      </c>
+      <c r="F136" t="s">
+        <v>12</v>
+      </c>
+      <c r="G136" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
+        <v>594</v>
+      </c>
+      <c r="B137" t="s">
+        <v>595</v>
+      </c>
+      <c r="C137" t="s">
+        <v>596</v>
+      </c>
+      <c r="D137" t="s">
+        <v>183</v>
+      </c>
+      <c r="E137" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>598</v>
+      </c>
+      <c r="B138" t="s">
+        <v>599</v>
+      </c>
+      <c r="C138" t="s">
+        <v>600</v>
+      </c>
+      <c r="D138" t="s">
+        <v>601</v>
+      </c>
+      <c r="E138" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" t="s">
+        <v>30</v>
+      </c>
+      <c r="G138" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>603</v>
+      </c>
+      <c r="B139" t="s">
+        <v>458</v>
+      </c>
+      <c r="C139" t="s">
+        <v>604</v>
+      </c>
+      <c r="D139" t="s">
+        <v>50</v>
+      </c>
+      <c r="E139" t="s">
+        <v>18</v>
+      </c>
+      <c r="F139" t="s">
+        <v>12</v>
+      </c>
+      <c r="G139" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
+        <v>606</v>
+      </c>
+      <c r="B140" t="s">
+        <v>226</v>
+      </c>
+      <c r="C140" t="s">
+        <v>607</v>
+      </c>
+      <c r="D140" t="s">
+        <v>345</v>
+      </c>
+      <c r="E140" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" t="s">
+        <v>12</v>
+      </c>
+      <c r="G140" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
+        <v>609</v>
+      </c>
+      <c r="B141" t="s">
+        <v>610</v>
+      </c>
+      <c r="C141" t="s">
+        <v>611</v>
+      </c>
+      <c r="D141" t="s">
+        <v>407</v>
+      </c>
+      <c r="E141" t="s">
+        <v>18</v>
+      </c>
+      <c r="F141" t="s">
+        <v>30</v>
+      </c>
+      <c r="G141" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
+        <v>613</v>
+      </c>
+      <c r="B142" t="s">
+        <v>614</v>
+      </c>
+      <c r="C142" t="s">
+        <v>615</v>
+      </c>
+      <c r="D142" t="s">
+        <v>364</v>
+      </c>
+      <c r="E142" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" t="s">
+        <v>30</v>
+      </c>
+      <c r="G142" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
+        <v>617</v>
+      </c>
+      <c r="B143" t="s">
+        <v>618</v>
+      </c>
+      <c r="C143" t="s">
+        <v>619</v>
+      </c>
+      <c r="D143" t="s">
+        <v>188</v>
+      </c>
+      <c r="E143" t="s">
+        <v>18</v>
+      </c>
+      <c r="F143" t="s">
+        <v>30</v>
+      </c>
+      <c r="G143" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" t="s">
+        <v>621</v>
+      </c>
+      <c r="B144" t="s">
+        <v>622</v>
+      </c>
+      <c r="C144" t="s">
+        <v>623</v>
+      </c>
+      <c r="D144" t="s">
+        <v>624</v>
+      </c>
+      <c r="E144" t="s">
+        <v>24</v>
+      </c>
+      <c r="F144" t="s">
+        <v>30</v>
+      </c>
+      <c r="G144" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>626</v>
+      </c>
+      <c r="B145" t="s">
+        <v>627</v>
+      </c>
+      <c r="C145" t="s">
+        <v>628</v>
+      </c>
+      <c r="D145" t="s">
+        <v>629</v>
+      </c>
+      <c r="E145" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" t="s">
+        <v>12</v>
+      </c>
+      <c r="G145" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>631</v>
+      </c>
+      <c r="B146" t="s">
+        <v>632</v>
+      </c>
+      <c r="C146" t="s">
+        <v>633</v>
+      </c>
+      <c r="D146" t="s">
+        <v>497</v>
+      </c>
+      <c r="E146" t="s">
+        <v>18</v>
+      </c>
+      <c r="F146" t="s">
+        <v>12</v>
+      </c>
+      <c r="G146" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>23</v>
+      </c>
+      <c r="B147" t="s">
+        <v>635</v>
+      </c>
+      <c r="C147" t="s">
+        <v>636</v>
+      </c>
+      <c r="D147" t="s">
+        <v>69</v>
+      </c>
+      <c r="E147" t="s">
+        <v>18</v>
+      </c>
+      <c r="F147" t="s">
+        <v>12</v>
+      </c>
+      <c r="G147" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>638</v>
+      </c>
+      <c r="B148" t="s">
+        <v>639</v>
+      </c>
+      <c r="C148" t="s">
+        <v>640</v>
+      </c>
+      <c r="D148" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" t="s">
+        <v>18</v>
+      </c>
+      <c r="F148" t="s">
+        <v>30</v>
+      </c>
+      <c r="G148" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>642</v>
+      </c>
+      <c r="B149" t="s">
+        <v>643</v>
+      </c>
+      <c r="C149" t="s">
+        <v>478</v>
+      </c>
+      <c r="D149" t="s">
+        <v>69</v>
+      </c>
+      <c r="E149" t="s">
+        <v>11</v>
+      </c>
+      <c r="F149" t="s">
+        <v>12</v>
+      </c>
+      <c r="G149" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>644</v>
+      </c>
+      <c r="B150" t="s">
+        <v>645</v>
+      </c>
+      <c r="C150" t="s">
+        <v>646</v>
+      </c>
+      <c r="D150" t="s">
+        <v>40</v>
+      </c>
+      <c r="E150" t="s">
+        <v>11</v>
+      </c>
+      <c r="F150" t="s">
+        <v>12</v>
+      </c>
+      <c r="G150" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>648</v>
+      </c>
+      <c r="B151" t="s">
+        <v>649</v>
+      </c>
+      <c r="C151" t="s">
+        <v>650</v>
+      </c>
+      <c r="D151" t="s">
+        <v>624</v>
+      </c>
+      <c r="E151" t="s">
+        <v>24</v>
+      </c>
+      <c r="F151" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>652</v>
+      </c>
+      <c r="B152" t="s">
+        <v>653</v>
+      </c>
+      <c r="C152" t="s">
+        <v>215</v>
+      </c>
+      <c r="D152" t="s">
+        <v>265</v>
+      </c>
+      <c r="E152" t="s">
+        <v>18</v>
+      </c>
+      <c r="F152" t="s">
+        <v>30</v>
+      </c>
+      <c r="G152" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>655</v>
+      </c>
+      <c r="B153" t="s">
+        <v>656</v>
+      </c>
+      <c r="C153" t="s">
+        <v>657</v>
+      </c>
+      <c r="D153" t="s">
+        <v>250</v>
+      </c>
+      <c r="E153" t="s">
+        <v>18</v>
+      </c>
+      <c r="F153" t="s">
+        <v>12</v>
+      </c>
+      <c r="G153" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>659</v>
+      </c>
+      <c r="B154" t="s">
+        <v>660</v>
+      </c>
+      <c r="C154" t="s">
+        <v>554</v>
+      </c>
+      <c r="D154" t="s">
+        <v>169</v>
+      </c>
+      <c r="E154" t="s">
+        <v>18</v>
+      </c>
+      <c r="F154" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>662</v>
+      </c>
+      <c r="B155" t="s">
+        <v>663</v>
+      </c>
+      <c r="C155" t="s">
+        <v>664</v>
+      </c>
+      <c r="D155" t="s">
+        <v>64</v>
+      </c>
+      <c r="E155" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" t="s">
+        <v>12</v>
+      </c>
+      <c r="G155" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" t="s">
+        <v>666</v>
+      </c>
+      <c r="B156" t="s">
+        <v>343</v>
+      </c>
+      <c r="C156" t="s">
+        <v>667</v>
+      </c>
+      <c r="D156" t="s">
+        <v>237</v>
+      </c>
+      <c r="E156" t="s">
+        <v>18</v>
+      </c>
+      <c r="F156" t="s">
+        <v>12</v>
+      </c>
+      <c r="G156" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" t="s">
+        <v>331</v>
+      </c>
+      <c r="B157" t="s">
+        <v>669</v>
+      </c>
+      <c r="C157" t="s">
+        <v>670</v>
+      </c>
+      <c r="D157" t="s">
+        <v>35</v>
+      </c>
+      <c r="E157" t="s">
+        <v>24</v>
+      </c>
+      <c r="F157" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" t="s">
+        <v>672</v>
+      </c>
+      <c r="B158" t="s">
+        <v>673</v>
+      </c>
+      <c r="C158" t="s">
+        <v>674</v>
+      </c>
+      <c r="D158" t="s">
+        <v>260</v>
+      </c>
+      <c r="E158" t="s">
+        <v>24</v>
+      </c>
+      <c r="F158" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" t="s">
+        <v>676</v>
+      </c>
+      <c r="B159" t="s">
+        <v>677</v>
+      </c>
+      <c r="C159" t="s">
+        <v>352</v>
+      </c>
+      <c r="D159" t="s">
+        <v>103</v>
+      </c>
+      <c r="E159" t="s">
+        <v>24</v>
+      </c>
+      <c r="F159" t="s">
+        <v>30</v>
+      </c>
+      <c r="G159" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>538</v>
+      </c>
+      <c r="B160" t="s">
+        <v>679</v>
+      </c>
+      <c r="C160" t="s">
+        <v>680</v>
+      </c>
+      <c r="D160" t="s">
+        <v>514</v>
+      </c>
+      <c r="E160" t="s">
+        <v>11</v>
+      </c>
+      <c r="F160" t="s">
+        <v>30</v>
+      </c>
+      <c r="G160" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>682</v>
+      </c>
+      <c r="B161" t="s">
+        <v>683</v>
+      </c>
+      <c r="C161" t="s">
+        <v>684</v>
+      </c>
+      <c r="D161" t="s">
+        <v>183</v>
+      </c>
+      <c r="E161" t="s">
+        <v>18</v>
+      </c>
+      <c r="F161" t="s">
+        <v>12</v>
+      </c>
+      <c r="G161" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>243</v>
+      </c>
+      <c r="B162" t="s">
+        <v>300</v>
+      </c>
+      <c r="C162" t="s">
+        <v>686</v>
+      </c>
+      <c r="D162" t="s">
+        <v>69</v>
+      </c>
+      <c r="E162" t="s">
+        <v>24</v>
+      </c>
+      <c r="F162" t="s">
+        <v>12</v>
+      </c>
+      <c r="G162" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" t="s">
+        <v>688</v>
+      </c>
+      <c r="B163" t="s">
+        <v>689</v>
+      </c>
+      <c r="C163" t="s">
+        <v>690</v>
+      </c>
+      <c r="D163" t="s">
+        <v>160</v>
+      </c>
+      <c r="E163" t="s">
+        <v>11</v>
+      </c>
+      <c r="F163" t="s">
+        <v>12</v>
+      </c>
+      <c r="G163" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" t="s">
+        <v>511</v>
+      </c>
+      <c r="B164" t="s">
+        <v>692</v>
+      </c>
+      <c r="C164" t="s">
+        <v>693</v>
+      </c>
+      <c r="D164" t="s">
+        <v>558</v>
+      </c>
+      <c r="E164" t="s">
+        <v>18</v>
+      </c>
+      <c r="F164" t="s">
+        <v>12</v>
+      </c>
+      <c r="G164" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" t="s">
+        <v>250</v>
+      </c>
+      <c r="B165" t="s">
+        <v>695</v>
+      </c>
+      <c r="C165" t="s">
+        <v>696</v>
+      </c>
+      <c r="D165" t="s">
+        <v>150</v>
+      </c>
+      <c r="E165" t="s">
+        <v>11</v>
+      </c>
+      <c r="F165" t="s">
+        <v>12</v>
+      </c>
+      <c r="G165" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" t="s">
+        <v>698</v>
+      </c>
+      <c r="B166" t="s">
+        <v>699</v>
+      </c>
+      <c r="C166" t="s">
+        <v>700</v>
+      </c>
+      <c r="D166" t="s">
+        <v>232</v>
+      </c>
+      <c r="E166" t="s">
+        <v>18</v>
+      </c>
+      <c r="F166" t="s">
+        <v>12</v>
+      </c>
+      <c r="G166" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" t="s">
+        <v>357</v>
+      </c>
+      <c r="B167" t="s">
+        <v>702</v>
+      </c>
+      <c r="C167" t="s">
+        <v>703</v>
+      </c>
+      <c r="D167" t="s">
+        <v>237</v>
+      </c>
+      <c r="E167" t="s">
+        <v>18</v>
+      </c>
+      <c r="F167" t="s">
+        <v>12</v>
+      </c>
+      <c r="G167" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" t="s">
+        <v>613</v>
+      </c>
+      <c r="B168" t="s">
+        <v>705</v>
+      </c>
+      <c r="C168" t="s">
+        <v>706</v>
+      </c>
+      <c r="D168" t="s">
+        <v>93</v>
+      </c>
+      <c r="E168" t="s">
+        <v>11</v>
+      </c>
+      <c r="F168" t="s">
+        <v>30</v>
+      </c>
+      <c r="G168" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" t="s">
+        <v>708</v>
+      </c>
+      <c r="B169" t="s">
+        <v>709</v>
+      </c>
+      <c r="C169" t="s">
+        <v>710</v>
+      </c>
+      <c r="D169" t="s">
+        <v>128</v>
+      </c>
+      <c r="E169" t="s">
+        <v>18</v>
+      </c>
+      <c r="F169" t="s">
+        <v>30</v>
+      </c>
+      <c r="G169" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" t="s">
+        <v>485</v>
+      </c>
+      <c r="C170" t="s">
+        <v>712</v>
+      </c>
+      <c r="D170" t="s">
+        <v>148</v>
+      </c>
+      <c r="E170" t="s">
+        <v>18</v>
+      </c>
+      <c r="F170" t="s">
+        <v>30</v>
+      </c>
+      <c r="G170" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" t="s">
+        <v>714</v>
+      </c>
+      <c r="B171" t="s">
+        <v>715</v>
+      </c>
+      <c r="C171" t="s">
+        <v>716</v>
+      </c>
+      <c r="D171" t="s">
+        <v>717</v>
+      </c>
+      <c r="E171" t="s">
+        <v>11</v>
+      </c>
+      <c r="F171" t="s">
+        <v>12</v>
+      </c>
+      <c r="G171" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" t="s">
+        <v>719</v>
+      </c>
+      <c r="B172" t="s">
+        <v>720</v>
+      </c>
+      <c r="C172" t="s">
+        <v>721</v>
+      </c>
+      <c r="D172" t="s">
+        <v>563</v>
+      </c>
+      <c r="E172" t="s">
+        <v>18</v>
+      </c>
+      <c r="F172" t="s">
+        <v>12</v>
+      </c>
+      <c r="G172" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" t="s">
+        <v>723</v>
+      </c>
+      <c r="B173" t="s">
+        <v>724</v>
+      </c>
+      <c r="C173" t="s">
+        <v>725</v>
+      </c>
+      <c r="D173" t="s">
+        <v>284</v>
+      </c>
+      <c r="E173" t="s">
+        <v>11</v>
+      </c>
+      <c r="F173" t="s">
+        <v>12</v>
+      </c>
+      <c r="G173" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" t="s">
+        <v>205</v>
+      </c>
+      <c r="B174" t="s">
+        <v>727</v>
+      </c>
+      <c r="C174" t="s">
+        <v>728</v>
+      </c>
+      <c r="D174" t="s">
+        <v>23</v>
+      </c>
+      <c r="E174" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" t="s">
+        <v>30</v>
+      </c>
+      <c r="G174" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" t="s">
+        <v>730</v>
+      </c>
+      <c r="B175" t="s">
+        <v>731</v>
+      </c>
+      <c r="C175" t="s">
+        <v>732</v>
+      </c>
+      <c r="D175" t="s">
+        <v>248</v>
+      </c>
+      <c r="E175" t="s">
+        <v>11</v>
+      </c>
+      <c r="F175" t="s">
+        <v>30</v>
+      </c>
+      <c r="G175" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" t="s">
+        <v>734</v>
+      </c>
+      <c r="B176" t="s">
+        <v>735</v>
+      </c>
+      <c r="C176" t="s">
+        <v>736</v>
+      </c>
+      <c r="D176" t="s">
+        <v>199</v>
+      </c>
+      <c r="E176" t="s">
+        <v>11</v>
+      </c>
+      <c r="F176" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" t="s">
+        <v>738</v>
+      </c>
+      <c r="B177" t="s">
+        <v>590</v>
+      </c>
+      <c r="C177" t="s">
+        <v>739</v>
+      </c>
+      <c r="D177" t="s">
+        <v>740</v>
+      </c>
+      <c r="E177" t="s">
+        <v>24</v>
+      </c>
+      <c r="F177" t="s">
+        <v>30</v>
+      </c>
+      <c r="G177" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" t="s">
+        <v>742</v>
+      </c>
+      <c r="B178" t="s">
+        <v>743</v>
+      </c>
+      <c r="C178" t="s">
+        <v>744</v>
+      </c>
+      <c r="D178" t="s">
+        <v>745</v>
+      </c>
+      <c r="E178" t="s">
+        <v>24</v>
+      </c>
+      <c r="F178" t="s">
+        <v>30</v>
+      </c>
+      <c r="G178" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" t="s">
+        <v>708</v>
+      </c>
+      <c r="B179" t="s">
+        <v>747</v>
+      </c>
+      <c r="C179" t="s">
+        <v>748</v>
+      </c>
+      <c r="D179" t="s">
+        <v>688</v>
+      </c>
+      <c r="E179" t="s">
+        <v>11</v>
+      </c>
+      <c r="F179" t="s">
+        <v>30</v>
+      </c>
+      <c r="G179" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" t="s">
+        <v>750</v>
+      </c>
+      <c r="B180" t="s">
+        <v>131</v>
+      </c>
+      <c r="C180" t="s">
+        <v>751</v>
+      </c>
+      <c r="D180" t="s">
+        <v>487</v>
+      </c>
+      <c r="E180" t="s">
+        <v>24</v>
+      </c>
+      <c r="F180" t="s">
+        <v>12</v>
+      </c>
+      <c r="G180" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" t="s">
+        <v>753</v>
+      </c>
+      <c r="B181" t="s">
+        <v>754</v>
+      </c>
+      <c r="C181" t="s">
+        <v>755</v>
+      </c>
+      <c r="D181" t="s">
+        <v>146</v>
+      </c>
+      <c r="E181" t="s">
+        <v>18</v>
+      </c>
+      <c r="F181" t="s">
+        <v>30</v>
+      </c>
+      <c r="G181" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" t="s">
+        <v>757</v>
+      </c>
+      <c r="B182" t="s">
+        <v>758</v>
+      </c>
+      <c r="C182" t="s">
+        <v>759</v>
+      </c>
+      <c r="D182" t="s">
+        <v>59</v>
+      </c>
+      <c r="E182" t="s">
+        <v>11</v>
+      </c>
+      <c r="F182" t="s">
+        <v>30</v>
+      </c>
+      <c r="G182" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" t="s">
+        <v>761</v>
+      </c>
+      <c r="B183" t="s">
+        <v>762</v>
+      </c>
+      <c r="C183" t="s">
+        <v>763</v>
+      </c>
+      <c r="D183" t="s">
+        <v>465</v>
+      </c>
+      <c r="E183" t="s">
+        <v>18</v>
+      </c>
+      <c r="F183" t="s">
+        <v>30</v>
+      </c>
+      <c r="G183" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" t="s">
+        <v>765</v>
+      </c>
+      <c r="B184" t="s">
+        <v>766</v>
+      </c>
+      <c r="C184" t="s">
+        <v>767</v>
+      </c>
+      <c r="D184" t="s">
+        <v>768</v>
+      </c>
+      <c r="E184" t="s">
+        <v>24</v>
+      </c>
+      <c r="F184" t="s">
+        <v>30</v>
+      </c>
+      <c r="G184" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" t="s">
+        <v>116</v>
+      </c>
+      <c r="B185" t="s">
+        <v>770</v>
+      </c>
+      <c r="C185" t="s">
+        <v>771</v>
+      </c>
+      <c r="D185" t="s">
+        <v>745</v>
+      </c>
+      <c r="E185" t="s">
+        <v>24</v>
+      </c>
+      <c r="F185" t="s">
+        <v>30</v>
+      </c>
+      <c r="G185" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" t="s">
+        <v>773</v>
+      </c>
+      <c r="B186" t="s">
+        <v>774</v>
+      </c>
+      <c r="C186" t="s">
+        <v>775</v>
+      </c>
+      <c r="D186" t="s">
+        <v>450</v>
+      </c>
+      <c r="E186" t="s">
+        <v>18</v>
+      </c>
+      <c r="F186" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" t="s">
+        <v>336</v>
+      </c>
+      <c r="B187" t="s">
+        <v>244</v>
+      </c>
+      <c r="C187" t="s">
+        <v>777</v>
+      </c>
+      <c r="D187" t="s">
+        <v>369</v>
+      </c>
+      <c r="E187" t="s">
+        <v>18</v>
+      </c>
+      <c r="F187" t="s">
+        <v>30</v>
+      </c>
+      <c r="G187" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" t="s">
+        <v>779</v>
+      </c>
+      <c r="B188" t="s">
+        <v>268</v>
+      </c>
+      <c r="C188" t="s">
+        <v>780</v>
+      </c>
+      <c r="D188" t="s">
+        <v>260</v>
+      </c>
+      <c r="E188" t="s">
+        <v>24</v>
+      </c>
+      <c r="F188" t="s">
+        <v>30</v>
+      </c>
+      <c r="G188" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" t="s">
+        <v>782</v>
+      </c>
+      <c r="B189" t="s">
+        <v>783</v>
+      </c>
+      <c r="C189" t="s">
+        <v>784</v>
+      </c>
+      <c r="D189" t="s">
+        <v>497</v>
+      </c>
+      <c r="E189" t="s">
+        <v>24</v>
+      </c>
+      <c r="F189" t="s">
+        <v>30</v>
+      </c>
+      <c r="G189" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7">
+      <c r="A190" t="s">
+        <v>786</v>
+      </c>
+      <c r="B190" t="s">
+        <v>787</v>
+      </c>
+      <c r="C190" t="s">
+        <v>788</v>
+      </c>
+      <c r="D190" t="s">
+        <v>789</v>
+      </c>
+      <c r="E190" t="s">
+        <v>24</v>
+      </c>
+      <c r="F190" t="s">
+        <v>12</v>
+      </c>
+      <c r="G190" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
+      <c r="A191" t="s">
+        <v>791</v>
+      </c>
+      <c r="B191" t="s">
+        <v>792</v>
+      </c>
+      <c r="C191" t="s">
+        <v>793</v>
+      </c>
+      <c r="D191" t="s">
+        <v>148</v>
+      </c>
+      <c r="E191" t="s">
+        <v>24</v>
+      </c>
+      <c r="F191" t="s">
+        <v>12</v>
+      </c>
+      <c r="G191" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7">
+      <c r="A192" t="s">
+        <v>795</v>
+      </c>
+      <c r="B192" t="s">
+        <v>796</v>
+      </c>
+      <c r="C192" t="s">
+        <v>177</v>
+      </c>
+      <c r="D192" t="s">
+        <v>745</v>
+      </c>
+      <c r="E192" t="s">
+        <v>18</v>
+      </c>
+      <c r="F192" t="s">
+        <v>30</v>
+      </c>
+      <c r="G192" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193" t="s">
+        <v>798</v>
+      </c>
+      <c r="B193" t="s">
+        <v>799</v>
+      </c>
+      <c r="C193" t="s">
+        <v>582</v>
+      </c>
+      <c r="D193" t="s">
+        <v>603</v>
+      </c>
+      <c r="E193" t="s">
+        <v>11</v>
+      </c>
+      <c r="F193" t="s">
+        <v>30</v>
+      </c>
+      <c r="G193" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7">
+      <c r="A194" t="s">
+        <v>801</v>
+      </c>
+      <c r="B194" t="s">
+        <v>656</v>
+      </c>
+      <c r="C194" t="s">
+        <v>802</v>
+      </c>
+      <c r="D194" t="s">
+        <v>803</v>
+      </c>
+      <c r="E194" t="s">
+        <v>11</v>
+      </c>
+      <c r="F194" t="s">
+        <v>12</v>
+      </c>
+      <c r="G194" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
+      <c r="A195" t="s">
+        <v>805</v>
+      </c>
+      <c r="B195" t="s">
+        <v>645</v>
+      </c>
+      <c r="C195" t="s">
+        <v>806</v>
+      </c>
+      <c r="D195" t="s">
+        <v>109</v>
+      </c>
+      <c r="E195" t="s">
+        <v>11</v>
+      </c>
+      <c r="F195" t="s">
+        <v>30</v>
+      </c>
+      <c r="G195" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196" t="s">
+        <v>568</v>
+      </c>
+      <c r="B196" t="s">
+        <v>808</v>
+      </c>
+      <c r="C196" t="s">
+        <v>164</v>
+      </c>
+      <c r="D196" t="s">
+        <v>69</v>
+      </c>
+      <c r="E196" t="s">
+        <v>11</v>
+      </c>
+      <c r="F196" t="s">
+        <v>30</v>
+      </c>
+      <c r="G196" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" t="s">
+        <v>810</v>
+      </c>
+      <c r="B197" t="s">
+        <v>811</v>
+      </c>
+      <c r="C197" t="s">
+        <v>684</v>
+      </c>
+      <c r="D197" t="s">
+        <v>487</v>
+      </c>
+      <c r="E197" t="s">
+        <v>18</v>
+      </c>
+      <c r="F197" t="s">
+        <v>12</v>
+      </c>
+      <c r="G197" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" t="s">
+        <v>813</v>
+      </c>
+      <c r="B198" t="s">
+        <v>814</v>
+      </c>
+      <c r="C198" t="s">
+        <v>815</v>
+      </c>
+      <c r="D198" t="s">
+        <v>64</v>
+      </c>
+      <c r="E198" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" t="s">
+        <v>12</v>
+      </c>
+      <c r="G198" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" t="s">
+        <v>817</v>
+      </c>
+      <c r="B199" t="s">
+        <v>818</v>
+      </c>
+      <c r="C199" t="s">
+        <v>434</v>
+      </c>
+      <c r="D199" t="s">
+        <v>79</v>
+      </c>
+      <c r="E199" t="s">
+        <v>24</v>
+      </c>
+      <c r="F199" t="s">
+        <v>30</v>
+      </c>
+      <c r="G199" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" t="s">
+        <v>820</v>
+      </c>
+      <c r="B200" t="s">
+        <v>821</v>
+      </c>
+      <c r="C200" t="s">
+        <v>822</v>
+      </c>
+      <c r="D200" t="s">
+        <v>823</v>
+      </c>
+      <c r="E200" t="s">
+        <v>11</v>
+      </c>
+      <c r="F200" t="s">
+        <v>30</v>
+      </c>
+      <c r="G200" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" t="s">
+        <v>825</v>
+      </c>
+      <c r="B201" t="s">
+        <v>826</v>
+      </c>
+      <c r="C201" t="s">
+        <v>827</v>
+      </c>
+      <c r="D201" t="s">
+        <v>382</v>
+      </c>
+      <c r="E201" t="s">
+        <v>11</v>
+      </c>
+      <c r="F201" t="s">
+        <v>12</v>
+      </c>
+      <c r="G201" t="s">
+        <v>828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>